<commit_message>
Atualiza Monte e Patos
</commit_message>
<xml_diff>
--- a/Monte/importarMonte.xlsx
+++ b/Monte/importarMonte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgugovbr-my.sharepoint.com/personal/pedro_guimaraes_cgu_gov_br/Documents/Pedro/PPGGO/MODELO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgugovbr-my.sharepoint.com/personal/pedro_guimaraes_cgu_gov_br/Documents/Pedro/PPGGO/MODELO/Monte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{DAE8B9E6-7CCD-4F8B-BF80-984490CB1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{409268FA-C2DB-4156-81EA-D1D4BDDB00BD}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="8_{DAE8B9E6-7CCD-4F8B-BF80-984490CB1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E1F5F8-3EBB-40D4-BB05-9D9DE3454739}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D33BA194-2E5A-46CB-BF13-D006A9E4191B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D33BA194-2E5A-46CB-BF13-D006A9E4191B}"/>
   </bookViews>
   <sheets>
     <sheet name="unidades" sheetId="1" r:id="rId1"/>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE730446-7824-4116-9627-BA51844BEEE0}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="1">
         <v>32</v>
@@ -913,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BD36B9-6FBB-45BA-A574-F9F17B544986}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualiza arquivos de Monte Carmelo e Patos de Minas
</commit_message>
<xml_diff>
--- a/Monte/importarMonte.xlsx
+++ b/Monte/importarMonte.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgugovbr-my.sharepoint.com/personal/pedro_guimaraes_cgu_gov_br/Documents/Pedro/PPGGO/MODELO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgugovbr-my.sharepoint.com/personal/pedro_guimaraes_cgu_gov_br/Documents/Pedro/PPGGO/MODELO/Monte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1190" documentId="8_{DAE8B9E6-7CCD-4F8B-BF80-984490CB1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0104DA-16E0-4B49-BF45-AF2D708D8EDD}"/>
+  <xr:revisionPtr revIDLastSave="1200" documentId="8_{DAE8B9E6-7CCD-4F8B-BF80-984490CB1294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E2B7F0-88D3-495B-8DC1-4B00C5709608}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D33BA194-2E5A-46CB-BF13-D006A9E4191B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D33BA194-2E5A-46CB-BF13-D006A9E4191B}"/>
   </bookViews>
   <sheets>
     <sheet name="unidades" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="92">
   <si>
     <t>Unidade</t>
   </si>
@@ -395,6 +395,15 @@
   </si>
   <si>
     <t>Exemplo certo</t>
+  </si>
+  <si>
+    <t>conector</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>==</t>
   </si>
 </sst>
 </file>
@@ -588,9 +597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -650,6 +656,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,8 +1148,8 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1170,7 +1177,7 @@
       <c r="F1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>29</v>
       </c>
       <c r="H1" s="19" t="s">
@@ -1187,576 +1194,576 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>144</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="23">
         <f>G2/2+H2/2+K2/2+I2*1.25+J2*2</f>
         <v>17</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="23">
         <f>SUM(G2:K2)</f>
         <v>34</v>
       </c>
-      <c r="E2" s="23">
-        <v>0</v>
-      </c>
-      <c r="F2" s="23">
+      <c r="E2" s="22">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22">
         <v>1</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="25">
         <v>12</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="22">
         <v>22</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>24</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <f t="shared" ref="C3:C11" si="0">G3/2+H3/2+K3/2+I3*1.25+J3*2</f>
         <v>0</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <f t="shared" ref="D3:D11" si="1">SUM(G3:K3)</f>
         <v>0</v>
       </c>
-      <c r="E3" s="23">
-        <v>0</v>
-      </c>
-      <c r="F3" s="23">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="E3" s="22">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>84</v>
       </c>
-      <c r="C4" s="24">
+      <c r="C4" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E4" s="23">
-        <v>0</v>
-      </c>
-      <c r="F4" s="23">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
+      <c r="E4" s="22">
+        <v>0</v>
+      </c>
+      <c r="F4" s="22">
+        <v>0</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="23">
-        <v>89</v>
-      </c>
-      <c r="C5" s="24">
+      <c r="B5" s="22">
+        <v>91</v>
+      </c>
+      <c r="C5" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E5" s="23">
-        <v>0</v>
-      </c>
-      <c r="F5" s="23">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="E5" s="22">
+        <v>0</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="23">
-        <v>19</v>
-      </c>
-      <c r="C6" s="24">
+      <c r="B6" s="22">
+        <v>22</v>
+      </c>
+      <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E6" s="23">
-        <v>0</v>
-      </c>
-      <c r="F6" s="23">
-        <v>0</v>
-      </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="E6" s="22">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>378</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="23">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="E7" s="23">
-        <v>0</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="E7" s="22">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22">
         <v>3</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>32</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="22">
         <v>73</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="22">
         <v>16</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>12</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="23">
-        <v>0</v>
-      </c>
-      <c r="F8" s="23">
-        <v>0</v>
-      </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="E8" s="22">
+        <v>0</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>299</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="23">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="23">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="E9" s="23">
-        <v>0</v>
-      </c>
-      <c r="F9" s="23">
+      <c r="E9" s="22">
+        <v>0</v>
+      </c>
+      <c r="F9" s="22">
         <v>2</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="25">
         <v>20</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="22">
         <v>40</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>31</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="23">
-        <v>0</v>
-      </c>
-      <c r="F10" s="23">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="E10" s="22">
+        <v>0</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="23">
-        <v>34</v>
-      </c>
-      <c r="C11" s="24">
+      <c r="B11" s="22">
+        <v>32</v>
+      </c>
+      <c r="C11" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-      <c r="F11" s="23">
-        <v>0</v>
-      </c>
-      <c r="G11" s="26"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="E11" s="22">
+        <v>0</v>
+      </c>
+      <c r="F11" s="22">
+        <v>0</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -1772,10 +1779,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1783,235 +1790,253 @@
     <col min="2" max="9" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="20">
-        <v>0</v>
-      </c>
-      <c r="C2" s="20">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2">
         <v>16</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2">
         <v>24</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2">
         <v>10</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="20">
-        <v>0</v>
-      </c>
-      <c r="C3" s="20">
-        <v>0</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3">
         <v>10</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" s="20">
-        <v>0</v>
-      </c>
-      <c r="H3" s="20">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="I3" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="20">
-        <v>0</v>
-      </c>
-      <c r="C4" s="20">
-        <v>0</v>
-      </c>
-      <c r="D4" s="20">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>8</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4">
         <v>8</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4">
         <v>8</v>
       </c>
-      <c r="G4" s="20">
-        <v>0</v>
-      </c>
-      <c r="H4" s="20">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>6</v>
       </c>
-      <c r="I4" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="20">
-        <v>0</v>
-      </c>
-      <c r="D5" s="20">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20">
-        <v>0</v>
-      </c>
-      <c r="F5" s="20">
-        <v>0</v>
-      </c>
-      <c r="G5" s="20">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20">
-        <v>0</v>
-      </c>
-      <c r="I5" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="20">
-        <v>0</v>
-      </c>
-      <c r="C6" s="20">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="20">
-        <v>0</v>
-      </c>
-      <c r="E6" s="20">
-        <v>0</v>
-      </c>
-      <c r="F6" s="20">
-        <v>0</v>
-      </c>
-      <c r="G6" s="20">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20">
-        <v>0</v>
-      </c>
-      <c r="I6" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="20">
-        <v>0</v>
-      </c>
-      <c r="C7" s="20">
-        <v>0</v>
-      </c>
-      <c r="D7" s="20">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>18</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7">
         <v>12</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" s="20">
-        <v>0</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>3</v>
       </c>
-      <c r="I7" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8">
         <v>1.65</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8">
         <v>1.65</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8">
         <v>1.65</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8">
         <v>1.65</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8">
         <v>1.65</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8">
         <v>1.65</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8">
         <v>0.6</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8">
         <v>0.6</v>
       </c>
     </row>
@@ -3320,227 +3345,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="42"/>
       <c r="I19" s="1" t="s">
         <v>88</v>
       </c>
@@ -3549,265 +3574,265 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="I20" s="29" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="I20" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="J20" s="28" t="s">
+      <c r="J20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="L20" s="28" t="s">
+      <c r="L20" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="N20" s="29" t="s">
+      <c r="N20" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="O20" s="28" t="s">
+      <c r="O20" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="P20" s="28" t="s">
+      <c r="P20" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="Q20" s="28" t="s">
+      <c r="Q20" s="27" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="I21" s="28" t="s">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="I21" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="27">
+      <c r="J21" s="26">
         <v>1</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="30">
         <v>2</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="L21" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="N21" s="28" t="s">
+      <c r="N21" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="O21" s="27">
+      <c r="O21" s="26">
         <v>1</v>
       </c>
-      <c r="P21" s="37">
+      <c r="P21" s="36">
         <v>3</v>
       </c>
-      <c r="Q21" s="38" t="s">
+      <c r="Q21" s="37" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="I22" s="28" t="s">
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="I22" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="J22" s="30" t="s">
+      <c r="J22" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="K22" s="27">
+      <c r="K22" s="26">
         <v>1</v>
       </c>
-      <c r="L22" s="34">
+      <c r="L22" s="33">
         <v>4</v>
       </c>
-      <c r="N22" s="28" t="s">
+      <c r="N22" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O22" s="36" t="s">
+      <c r="O22" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="P22" s="27">
+      <c r="P22" s="26">
         <v>1</v>
       </c>
-      <c r="Q22" s="28">
+      <c r="Q22" s="27">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="I23" s="28" t="s">
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="I23" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="32">
+      <c r="J23" s="31">
         <v>3</v>
       </c>
-      <c r="K23" s="35" t="s">
+      <c r="K23" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="26">
         <v>1</v>
       </c>
-      <c r="N23" s="28" t="s">
+      <c r="N23" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="O23" s="28">
+      <c r="O23" s="27">
         <v>3</v>
       </c>
-      <c r="P23" s="38" t="s">
+      <c r="P23" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="Q23" s="27">
+      <c r="Q23" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="N24" s="39" t="s">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="N24" s="38" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="43"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>